<commit_message>
Added Link Access date range to Excel sheet
</commit_message>
<xml_diff>
--- a/Exported_Case_Arrival_Final.xlsx
+++ b/Exported_Case_Arrival_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Corona Virus\Coronavirus-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5F389-D8F8-4135-9B29-5AA3B4F432BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBA64CE-17BD-44C7-BA85-555973966421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>Had minor symptoms on flight and hospitalized shortly after</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Reported to be aymptomatic at time of testing (wife of confirmed case), no indication if or when symptoms appeared</t>
+  </si>
+  <si>
+    <t>Reference (Date range links accessed: January 31, 2020 to Febraury 8, 2020)</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -801,7 +801,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -812,7 +812,7 @@
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -823,7 +823,7 @@
     </row>
     <row r="3" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
@@ -846,13 +846,13 @@
         <v>15</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -866,10 +866,10 @@
       <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
       <c r="F6" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>35</v>
@@ -905,10 +905,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
@@ -929,7 +929,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>42</v>
@@ -948,10 +948,10 @@
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>29</v>
@@ -999,10 +999,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -1024,7 +1024,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>38</v>
@@ -1075,10 +1075,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>67</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
@@ -1097,10 +1097,10 @@
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>49</v>
@@ -1131,7 +1131,7 @@
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>52</v>
@@ -1148,7 +1148,7 @@
       <c r="D18" s="13"/>
       <c r="E18" s="14"/>
       <c r="F18" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>37</v>
@@ -1175,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
@@ -1199,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>22</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
@@ -1271,7 +1271,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
@@ -1300,7 +1300,7 @@
         <v>24</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" s="16" t="s">
         <v>48</v>
@@ -1348,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>44</v>
@@ -1372,10 +1372,10 @@
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="28" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1394,10 +1394,10 @@
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1448,7 +1448,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
@@ -1476,7 +1476,7 @@
         <v>19</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -1505,7 +1505,7 @@
         <v>18</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
@@ -1534,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -1563,7 +1563,7 @@
         <v>17</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -1587,7 +1587,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>46</v>
@@ -1609,7 +1609,7 @@
       <c r="D36" s="13"/>
       <c r="E36" s="14"/>
       <c r="F36" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>56</v>
@@ -1636,7 +1636,7 @@
         <v>28</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -1665,7 +1665,7 @@
         <v>27</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
@@ -1694,7 +1694,7 @@
         <v>27</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
@@ -1723,7 +1723,7 @@
         <v>57</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
@@ -1752,7 +1752,7 @@
         <v>58</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
@@ -1778,10 +1778,10 @@
         <v>3</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H42" s="27"/>
       <c r="I42" s="27"/>
@@ -1810,7 +1810,7 @@
         <v>26</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -1834,7 +1834,7 @@
         <v>-3</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>36</v>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>40</v>
@@ -1875,7 +1875,7 @@
       <c r="D46" s="13"/>
       <c r="E46" s="14"/>
       <c r="F46" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>54</v>
@@ -1892,7 +1892,7 @@
       <c r="D47" s="13"/>
       <c r="E47" s="14"/>
       <c r="F47" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>51</v>
@@ -1914,10 +1914,10 @@
         <v>4</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H48" s="27"/>
       <c r="I48" s="27"/>
@@ -1941,10 +1941,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>

</xml_diff>

<commit_message>
Updated outputprob and adjusted column width
</commit_message>
<xml_diff>
--- a/Exported_Case_Arrival_Final.xlsx
+++ b/Exported_Case_Arrival_Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Corona Virus\Coronavirus-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBA64CE-17BD-44C7-BA85-555973966421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32FC346-1951-45AA-B18D-3D7385FA644C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,7 +793,7 @@
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="209.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="255.42578125" customWidth="1"/>
     <col min="8" max="16384" width="14.42578125" style="24"/>

</xml_diff>

<commit_message>
Corrected spelling in Table
</commit_message>
<xml_diff>
--- a/Exported_Case_Arrival_Final.xlsx
+++ b/Exported_Case_Arrival_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Corona Virus\Coronavirus-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32FC346-1951-45AA-B18D-3D7385FA644C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750E5FC4-DB0A-4B86-8DFE-0519DA75171A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,15 +113,6 @@
     <t>50 years old man, visited Wuhan from Dec-24 to Jan-13, confirmed with coronvirus on Jan-30</t>
   </si>
   <si>
-    <t xml:space="preserve"> a woman in her 50s, visited Wuhan Jan. 13-15, then traveled in Europe from Jan 16-25, cough start Jan. 22 and become worse on Jan. 25, Jan-25 arrived Taiwan and report to hospital and confirmed on Jan. 26;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> a woman in her 50s, worked in Wuhan since Oct, 2019, arrived Taiwan on Jan. 20, fever and muscle pain on Jan. 25, confirmed on Jan 27; Her husband showed symptoms on Jan. 26, confirmed on Jan. 28.</t>
-  </si>
-  <si>
-    <t>a man in his 40s, worked in Wuhan since Sept. 2019, returned to Taiwan on Jan 12, showed symptom on Jan. 21, diagnosed as common fever on Jan. 22, confirmed with coronvirus on Jan. 30.</t>
-  </si>
-  <si>
     <t>https://news.ontario.ca/mohltc/en/2020/01/ontario-confirms-first-case-of-wuhan-novel-coronavirus.html</t>
   </si>
   <si>
@@ -206,12 +197,6 @@
     <t>https://www.thelocal.se/20200131/first-case-of-coronavirus-confirmed-in-jonkoping-sweden</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2 person traveled from Wuhan to Taiwan on Jan. 21, doctor visit on Jan 23, confirmed on Jan. 24</t>
-  </si>
-  <si>
-    <t>Two woman in their 70s living in Wuhan, arrived Taiwan on Jan. 22, showed symptoms on Jan. 25, confirmed on Jan. 28;</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
     <t xml:space="preserve">Arrived in Ujjain on January 13 from Hubei province. Was kept in quaratine then moved to isolation. </t>
   </si>
   <si>
-    <t>32 yr old woamn from Wuhan. Flew  to Helsinki Airport and took a connecting flight to Ivalo Airport in Inari (potentially exposed 15 people)</t>
-  </si>
-  <si>
     <t>Student at Western University. Self-quaratined and exhibited mild symptoms and weakly positive</t>
   </si>
   <si>
@@ -317,15 +299,9 @@
     <t>This case was supposabley infected in Singapore (not used in the importation analysis since not travel to China)</t>
   </si>
   <si>
-    <t>Arrived with no symptoms and went to see GP one started to developl symptoms</t>
-  </si>
-  <si>
     <t>Grandmother fell ill and went to seek medical help on the Janaury 23, but unclear as to when symptoms first appeared</t>
   </si>
   <si>
-    <t>Reports indicate that the individual arrive a few days prior to symptoms. We conservatiely assumedtheyh arrived one day prior to confirmation.</t>
-  </si>
-  <si>
     <t>Began to feel unwell a few days after arrival, but no clear indication as to when symptom onset occurred (i.e. sore throat or cough)</t>
   </si>
   <si>
@@ -338,9 +314,6 @@
     <t>66 year old male experienced fever Janaury 17, son (who man met upon arrival) exhibit similar symoms on the 20th</t>
   </si>
   <si>
-    <t>Woman in 20's had visited Wuhan. Reported had no symptoms upon arrival . No duration between arrival and symptom onset. Since there was no date of symptom onset specified, we did not include in sypotmatic arrival analysis</t>
-  </si>
-  <si>
     <t>Time symptom onset uncertain</t>
   </si>
   <si>
@@ -348,6 +321,33 @@
   </si>
   <si>
     <t>Reference (Date range links accessed: January 31, 2020 to Febraury 8, 2020)</t>
+  </si>
+  <si>
+    <t>Woman in 20's had visited Wuhan. Reported had no symptoms upon arrival . No duration between arrival and symptom onset. Since there was no date of symptom onset specified, we did not include in symptomatic arrival analysis</t>
+  </si>
+  <si>
+    <t>A man in his 40s, worked in Wuhan since Sept. 2019, returned to Taiwan on Jan 12, showed symptom on Jan. 21, diagnosed as common fever on Jan. 22, confirmed with coronvirus on Jan. 30.</t>
+  </si>
+  <si>
+    <t>A woman in her 50s, worked in Wuhan since Oct, 2019, arrived Taiwan on Jan. 20, fever and muscle pain on Jan. 25, confirmed on Jan 27; Her husband showed symptoms on Jan. 26, confirmed on Jan. 28.</t>
+  </si>
+  <si>
+    <t>A woman in her 50s, visited Wuhan Jan. 13-15, then traveled in Europe from Jan 16-25, cough start Jan. 22 and become worse on Jan. 25, Jan-25 arrived Taiwan and report to hospital and confirmed on Jan. 26;</t>
+  </si>
+  <si>
+    <t>Reports indicate that the individual arrive a few days prior to symptoms. We conservatiely assumed they arrived one day prior to confirmation.</t>
+  </si>
+  <si>
+    <t>Person traveled from Wuhan to Taiwan on Jan. 21, doctor visit on Jan 23, confirmed on Jan. 24</t>
+  </si>
+  <si>
+    <t>Arrived with no symptoms and went to see GP once they started to develope symptoms</t>
+  </si>
+  <si>
+    <t>32 yr old woamn from Wuhan. Flew to Helsinki Airport and took a connecting flight to Ivalo Airport in Inari (potentially exposed 15 people)</t>
+  </si>
+  <si>
+    <t>Two women in their 70s living in Wuhan, arrived Taiwan on Jan. 22, showed symptoms on Jan. 25, confirmed on Jan. 28;</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -794,14 +794,18 @@
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="209.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="214.140625" customWidth="1"/>
     <col min="7" max="7" width="255.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="24"/>
+    <col min="8" max="9" width="14.42578125" style="24"/>
+    <col min="10" max="10" width="5.42578125" style="24" customWidth="1"/>
+    <col min="11" max="11" width="1.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="0.28515625" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -812,7 +816,7 @@
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -823,7 +827,7 @@
     </row>
     <row r="3" spans="1:12" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
@@ -832,7 +836,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:12" s="26" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="26" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -846,13 +850,13 @@
         <v>15</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -866,10 +870,10 @@
       <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -883,10 +887,10 @@
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
       <c r="F6" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -905,10 +909,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
@@ -918,7 +922,7 @@
     </row>
     <row r="8" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="13">
         <v>43853</v>
@@ -929,10 +933,10 @@
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -948,10 +952,10 @@
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -972,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
@@ -999,10 +1003,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
@@ -1021,10 +1025,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
@@ -1048,10 +1052,10 @@
         <v>3</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -1075,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
@@ -1097,15 +1101,15 @@
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="13">
         <v>43843</v>
@@ -1114,15 +1118,15 @@
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17" s="13">
         <v>43859</v>
@@ -1131,10 +1135,10 @@
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1148,10 +1152,10 @@
       <c r="D18" s="13"/>
       <c r="E18" s="14"/>
       <c r="F18" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1175,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
@@ -1199,7 +1203,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1218,7 +1222,7 @@
         <v>22</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1242,7 +1246,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
@@ -1271,7 +1275,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
@@ -1300,7 +1304,7 @@
         <v>24</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
@@ -1310,7 +1314,7 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" s="13">
         <v>43853</v>
@@ -1324,10 +1328,10 @@
         <v>6</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
@@ -1337,7 +1341,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="13">
         <v>43839</v>
@@ -1348,10 +1352,10 @@
         <v>4</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
@@ -1361,7 +1365,7 @@
     </row>
     <row r="27" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="13">
         <v>43851</v>
@@ -1372,10 +1376,10 @@
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
@@ -1385,7 +1389,7 @@
     </row>
     <row r="28" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1394,10 +1398,10 @@
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1416,10 +1420,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
@@ -1448,7 +1452,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
@@ -1476,7 +1480,7 @@
         <v>19</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -1505,7 +1509,7 @@
         <v>18</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
@@ -1534,7 +1538,7 @@
         <v>19</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -1563,7 +1567,7 @@
         <v>17</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -1573,7 +1577,7 @@
     </row>
     <row r="35" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B35" s="13">
         <v>43849</v>
@@ -1587,10 +1591,10 @@
         <v>6</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
@@ -1600,7 +1604,7 @@
     </row>
     <row r="36" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B36" s="13">
         <v>43854</v>
@@ -1609,10 +1613,10 @@
       <c r="D36" s="13"/>
       <c r="E36" s="14"/>
       <c r="F36" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -1633,10 +1637,10 @@
         <v>9</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
@@ -1662,10 +1666,10 @@
         <v>6</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
@@ -1691,10 +1695,10 @@
         <v>5</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
@@ -1720,10 +1724,10 @@
         <v>2</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
@@ -1749,10 +1753,10 @@
         <v>3</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
@@ -1778,10 +1782,10 @@
         <v>3</v>
       </c>
       <c r="F42" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="H42" s="27"/>
       <c r="I42" s="27"/>
@@ -1807,10 +1811,10 @@
         <v>-3</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -1834,10 +1838,10 @@
         <v>-3</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
@@ -1847,7 +1851,7 @@
     </row>
     <row r="45" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B45" s="13">
         <v>43846</v>
@@ -1858,15 +1862,15 @@
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" s="13">
         <v>43860</v>
@@ -1875,15 +1879,15 @@
       <c r="D46" s="13"/>
       <c r="E46" s="14"/>
       <c r="F46" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B47" s="13">
         <v>43843</v>
@@ -1892,15 +1896,15 @@
       <c r="D47" s="13"/>
       <c r="E47" s="14"/>
       <c r="F47" s="12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" s="15">
         <v>43845</v>
@@ -1914,10 +1918,10 @@
         <v>4</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H48" s="27"/>
       <c r="I48" s="27"/>
@@ -1941,10 +1945,10 @@
         <v>4</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>
@@ -2179,6 +2183,6 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="3" scale="33" fitToHeight="0" orientation="landscape" r:id="rId46"/>
+  <pageSetup paperSize="3" scale="35" fitToHeight="0" orientation="landscape" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>